<commit_message>
feat: release v2.0.0 - UI overhaul, notification center, and dynamic job queue
</commit_message>
<xml_diff>
--- a/excel_轉換/活頁簿1.xlsx
+++ b/excel_轉換/活頁簿1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\114年\辦公\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP_600_G1_2ND\Desktop\工作自動化\excel_轉換\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B4BA66-B57E-480A-8CDD-897ED7624258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C6D84E-B824-4AE7-BCEA-D76269E79F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>

</xml_diff>